<commit_message>
Deploy the implementation guide.
</commit_message>
<xml_diff>
--- a/ig/CodeSystem-analysis-request-code.xlsx
+++ b/ig/CodeSystem-analysis-request-code.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-01-30T21:30:05+00:00</t>
+    <t>2023-02-09T16:19:35+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Global Developmental Delay / Intellectual Deficiency (Trio)</t>
+  </si>
+  <si>
+    <t>RGDI+</t>
   </si>
 </sst>
 </file>
@@ -480,7 +483,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -596,6 +599,18 @@
       </c>
       <c r="D9" s="2"/>
     </row>
+    <row r="10">
+      <c r="A10" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>